<commit_message>
feat: Updated rubtric for Week3 presentations
</commit_message>
<xml_diff>
--- a/evaluation_rubrics/presentation_week3_rubric.xlsx
+++ b/evaluation_rubrics/presentation_week3_rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markjack/Desktop/GSU Fall 2024/Course MSA 8030 Data Communications/Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0912E0A-F837-304B-881D-81D0EC2D1B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C92F5B-D17B-194A-9B04-9870A49C9861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="1260" windowWidth="25900" windowHeight="18580" xr2:uid="{89AAD315-E4F2-4C41-BBED-5FFCAC1DB04B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Criteria</t>
   </si>
@@ -72,13 +72,31 @@
   </si>
   <si>
     <t>Quality and Relevance of Visualizations</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PowerPoint presentation is exceptional in design and delivery. Slides are cohesive with a consistent design, using appropriate fonts, colors, and objects. The presentation flows smoothly, is engaging, and keeps the audience's attention. The presenter delivers the content confidently and clearly within the allotted time slot. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PowerPoint presentation is well- designed and delivered. Slides exhibit a good degree of cohesion in terms of design elements. The presentation is clear and mostly fluent, and the presenter manages to stay within the allotted time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PowerPoint presentation lacks some cohesiveness in design elements, making it less visually appealing. The delivery is somewhat choppy but generally understandable, and the presentation mostly fits the allotted time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PowerPoint presentation is poorly designed, lacking consistency in fonts, colors, and objects. The delivery is disjointed or difficult to follow, and the presentation significantly exceeds or falls short of the allotted time. </t>
+  </si>
+  <si>
+    <t>Missing or no work was submitted.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +108,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -124,6 +149,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -440,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F6A9AB-1ED0-1E46-8E05-CDAC3033AB71}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,10 +482,11 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="21.83203125" style="3" customWidth="1"/>
     <col min="3" max="6" width="44" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="26" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -473,8 +505,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -482,7 +517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -490,7 +525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -498,7 +533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -506,12 +541,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Update WQeek 3 evaluation rubric
</commit_message>
<xml_diff>
--- a/evaluation_rubrics/presentation_week3_rubric.xlsx
+++ b/evaluation_rubrics/presentation_week3_rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markjack/Desktop/GSU Fall 2024/Course MSA 8030 Data Communications/Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markjack/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C92F5B-D17B-194A-9B04-9870A49C9861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED4EDD1-F656-8B4B-8CA2-EE0BA62398A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="1260" windowWidth="25900" windowHeight="18580" xr2:uid="{89AAD315-E4F2-4C41-BBED-5FFCAC1DB04B}"/>
+    <workbookView xWindow="0" yWindow="1620" windowWidth="25900" windowHeight="18580" xr2:uid="{89AAD315-E4F2-4C41-BBED-5FFCAC1DB04B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Criteria</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Description of Business/Project</t>
   </si>
   <si>
-    <t>Description of Core Business Processes</t>
-  </si>
-  <si>
     <t>Description and Completeness of Possible Use Cases</t>
   </si>
   <si>
@@ -90,6 +87,42 @@
   </si>
   <si>
     <t>Missing or no work was submitted.</t>
+  </si>
+  <si>
+    <t>An engaging and convincing story line is created describing the business, its challenges, the primary business problem to be solved and what resources are available, what constraints have to be considered, what costs and risks are involved. The description clearly follows the SMART steps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every use case is described clearly and concisely. Their relevance to solving the business problem clearly established. The outlines of their feasibility studies are sketched with timelines and a decision process to rank the use cases in terms feasibility and ability to create business value. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The visualization stands out in terms of quality, style, clarity, and its ability to focus the key messages in describing the business problem at hand. Color, graph choice, labeling, descriptions are thoughtfully and effectively </t>
+  </si>
+  <si>
+    <t>The visualization used was relevant, to the point and added key information to illustrate the business problem succinctly and clearly. It used space, color, the choice of graphing style and other elements professionally and effectively to add to the overall message.</t>
+  </si>
+  <si>
+    <t>A list of possible use cases is motivated well and connects directly with the business problem solution or aspects of it. A process of ranking the feasibility of each use case is outlined.</t>
+  </si>
+  <si>
+    <t>All aspects of the business problem are outlined, connected and form an understandable description of the main issue(s) of the company/project and the type of solution that is being desired by the stakeholders. Key aspects like resources, constraints, costs, and other requirements provide a complete picture.</t>
+  </si>
+  <si>
+    <t>A basic outline of the business problem is provided. But important details are missing. Or the description is not concise but dives into too many irrelevant details are provided that distract from explaining the main business problem that needs to be solved.</t>
+  </si>
+  <si>
+    <t>Use cases relevant to the business problem are mentioned. But their relative importance is not clear and/or key use cases are missing in the description.</t>
+  </si>
+  <si>
+    <t>A visualization was added that was useful to communicate the overall description of the business problem but the visual could have been improved to make points more clearly or was not used strategically to emphasize key points in the presentation.</t>
+  </si>
+  <si>
+    <t>The business problem is mentioned but not clearly outlined and the relevance of points made is not clear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The relevance of use cases described here in connection with the business problem at hand is not clear. </t>
+  </si>
+  <si>
+    <t>A visualization is included in the slide deck but only has limited relevance for the business problem discussion, key elements in the graph like axis labels are missing or hard to read.</t>
   </si>
 </sst>
 </file>
@@ -140,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -150,9 +183,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -471,10 +501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F6A9AB-1ED0-1E46-8E05-CDAC3033AB71}">
-  <dimension ref="A1:G6"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,65 +539,103 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="49" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: Upload Week 4 presenations rubric
</commit_message>
<xml_diff>
--- a/evaluation_rubrics/presentation_week3_rubric.xlsx
+++ b/evaluation_rubrics/presentation_week3_rubric.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markjack/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markjack/Desktop/GSU Fall 2024/Course MSA 8030 Data Communications/evaluation rubrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED4EDD1-F656-8B4B-8CA2-EE0BA62398A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C9675D-6440-1D40-9801-0F94B23D0EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1620" windowWidth="25900" windowHeight="18580" xr2:uid="{89AAD315-E4F2-4C41-BBED-5FFCAC1DB04B}"/>
+    <workbookView xWindow="3860" yWindow="860" windowWidth="25900" windowHeight="18580" xr2:uid="{89AAD315-E4F2-4C41-BBED-5FFCAC1DB04B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>